<commit_message>
AUTO FROM work 12.06.2024 15:46:19,02
</commit_message>
<xml_diff>
--- a/media/1.xlsx
+++ b/media/1.xlsx
@@ -440,6 +440,11 @@
           <t>Разр. ПО для моб. Платформ ФМЕ ПОИТ3 ЗФПО</t>
         </is>
       </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>210</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="C5" t="inlineStr">
@@ -465,7 +470,11 @@
           <t>СПП (ЗО) 2 курс колония</t>
         </is>
       </c>
-      <c r="E6" s="1" t="n"/>
+      <c r="E6" s="1" t="inlineStr">
+        <is>
+          <t>115</t>
+        </is>
+      </c>
       <c r="F6" s="1" t="n"/>
       <c r="G6" s="1" t="n"/>
       <c r="H6" s="1" t="n"/>

</xml_diff>

<commit_message>
AUTO FROM work 12.06.2024 15:57:46,27
</commit_message>
<xml_diff>
--- a/media/1.xlsx
+++ b/media/1.xlsx
@@ -9,7 +9,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -25,21 +25,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="1">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -47,13 +41,233 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -421,624 +635,666 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B4:H60"/>
+  <dimension ref="A4:H60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:H21"/>
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="12" customWidth="1" style="1" min="3" max="3"/>
+    <col width="45.28515625" customWidth="1" style="1" min="4" max="4"/>
+  </cols>
   <sheetData>
+    <row r="1" ht="4.5" customHeight="1" s="1"/>
+    <row r="2" ht="3.75" customHeight="1" s="1"/>
+    <row r="3" ht="5.25" customHeight="1" s="1" thickBot="1"/>
     <row r="4">
-      <c r="C4" t="inlineStr">
+      <c r="B4" s="26" t="inlineStr">
+        <is>
+          <t>ПОНЕДЕЛЬНИК</t>
+        </is>
+      </c>
+      <c r="C4" s="18" t="inlineStr">
         <is>
           <t>08:15-09:35</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="D4" s="19" t="inlineStr">
         <is>
           <t>Разр. ПО для моб. Платформ ФМЕ ПОИТ3 ЗФПО</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="E4" s="20" t="inlineStr">
         <is>
           <t>210</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="C5" t="inlineStr">
+      <c r="B5" s="27" t="n"/>
+      <c r="C5" s="21" t="inlineStr">
         <is>
           <t>09:50-11:10</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="D5" s="6" t="inlineStr">
         <is>
           <t>Резерв</t>
         </is>
       </c>
+      <c r="E5" s="22" t="n"/>
     </row>
     <row r="6">
-      <c r="B6" s="1" t="n"/>
-      <c r="C6" s="1" t="inlineStr">
+      <c r="B6" s="27" t="n"/>
+      <c r="C6" s="21" t="inlineStr">
         <is>
           <t>11:25-12:45</t>
         </is>
       </c>
-      <c r="D6" s="1" t="inlineStr">
+      <c r="D6" s="6" t="inlineStr">
         <is>
           <t>СПП (ЗО) 2 курс колония</t>
         </is>
       </c>
-      <c r="E6" s="1" t="inlineStr">
+      <c r="E6" s="22" t="inlineStr">
         <is>
           <t>115</t>
         </is>
       </c>
-      <c r="F6" s="1" t="n"/>
-      <c r="G6" s="1" t="n"/>
-      <c r="H6" s="1" t="n"/>
     </row>
     <row r="7">
-      <c r="B7" s="1" t="n"/>
-      <c r="C7" s="1" t="inlineStr">
+      <c r="B7" s="27" t="n"/>
+      <c r="C7" s="21" t="inlineStr">
         <is>
           <t>13:15-14:35</t>
         </is>
       </c>
-      <c r="D7" s="1" t="inlineStr">
-        <is>
-          <t>Пусто</t>
-        </is>
-      </c>
-      <c r="E7" s="1" t="n"/>
-      <c r="F7" s="1" t="n"/>
-      <c r="G7" s="1" t="n"/>
-      <c r="H7" s="1" t="n"/>
+      <c r="D7" s="6" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
+      <c r="E7" s="22" t="n"/>
     </row>
     <row r="8">
-      <c r="B8" s="1" t="n"/>
-      <c r="C8" s="1" t="inlineStr">
+      <c r="B8" s="27" t="n"/>
+      <c r="C8" s="21" t="inlineStr">
         <is>
           <t>14:50-16:10</t>
         </is>
       </c>
-      <c r="D8" s="1" t="inlineStr">
-        <is>
-          <t>Пусто</t>
-        </is>
-      </c>
-      <c r="E8" s="1" t="n"/>
-      <c r="F8" s="1" t="n"/>
-      <c r="G8" s="1" t="n"/>
-      <c r="H8" s="1" t="n"/>
+      <c r="D8" s="6" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
+      <c r="E8" s="22" t="n"/>
     </row>
     <row r="9">
-      <c r="B9" s="1" t="n"/>
-      <c r="C9" s="1" t="inlineStr">
+      <c r="B9" s="27" t="n"/>
+      <c r="C9" s="21" t="inlineStr">
         <is>
           <t>16:40-18:00</t>
         </is>
       </c>
-      <c r="D9" s="1" t="inlineStr">
-        <is>
-          <t>Пусто</t>
-        </is>
-      </c>
-      <c r="E9" s="1" t="n"/>
-      <c r="F9" s="1" t="n"/>
-      <c r="G9" s="1" t="n"/>
-      <c r="H9" s="1" t="n"/>
-    </row>
-    <row r="10">
-      <c r="B10" s="1" t="n"/>
-      <c r="C10" s="1" t="inlineStr">
+      <c r="D9" s="6" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
+      <c r="E9" s="22" t="n"/>
+    </row>
+    <row r="10" ht="15.75" customHeight="1" s="1" thickBot="1">
+      <c r="B10" s="28" t="n"/>
+      <c r="C10" s="23" t="inlineStr">
         <is>
           <t>18:10-19:30</t>
         </is>
       </c>
-      <c r="D10" s="1" t="inlineStr">
-        <is>
-          <t>Пусто</t>
-        </is>
-      </c>
-      <c r="E10" s="1" t="n"/>
-      <c r="F10" s="1" t="n"/>
-      <c r="G10" s="1" t="n"/>
-      <c r="H10" s="1" t="n"/>
-    </row>
-    <row r="11">
-      <c r="B11" s="1" t="n"/>
-      <c r="C11" s="1" t="n"/>
-      <c r="D11" s="1" t="n"/>
-      <c r="E11" s="1" t="n"/>
-      <c r="F11" s="1" t="n"/>
-      <c r="G11" s="1" t="n"/>
-      <c r="H11" s="1" t="n"/>
-    </row>
-    <row r="12">
-      <c r="B12" s="1" t="n"/>
-      <c r="C12" s="1" t="n"/>
-      <c r="D12" s="1" t="n"/>
-      <c r="E12" s="1" t="n"/>
-      <c r="F12" s="1" t="n"/>
-      <c r="G12" s="1" t="n"/>
-      <c r="H12" s="1" t="n"/>
-    </row>
-    <row r="13">
-      <c r="B13" s="1" t="n"/>
-      <c r="C13" s="1" t="n"/>
-      <c r="D13" s="1" t="n"/>
-      <c r="E13" s="1" t="n"/>
-      <c r="F13" s="1" t="n"/>
-      <c r="G13" s="1" t="n"/>
-      <c r="H13" s="1" t="n"/>
-    </row>
+      <c r="D10" s="24" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
+      <c r="E10" s="25" t="n"/>
+    </row>
+    <row r="11" ht="3.75" customHeight="1" s="1"/>
+    <row r="12" ht="4.5" customHeight="1" s="1"/>
+    <row r="13" ht="4.5" customHeight="1" s="1" thickBot="1"/>
     <row r="14">
-      <c r="B14" s="1" t="n"/>
-      <c r="C14" s="1" t="inlineStr">
+      <c r="B14" s="26" t="inlineStr">
+        <is>
+          <t>ВТОРНИК</t>
+        </is>
+      </c>
+      <c r="C14" s="18" t="inlineStr">
         <is>
           <t>08:15-09:35</t>
         </is>
       </c>
-      <c r="D14" s="1" t="inlineStr">
-        <is>
-          <t>Пусто</t>
-        </is>
-      </c>
-      <c r="E14" s="1" t="n"/>
-      <c r="F14" s="1" t="n"/>
-      <c r="G14" s="1" t="n"/>
-      <c r="H14" s="1" t="n"/>
+      <c r="D14" s="19" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
+      <c r="E14" s="20" t="n"/>
     </row>
     <row r="15">
-      <c r="B15" s="1" t="n"/>
-      <c r="C15" s="1" t="inlineStr">
+      <c r="B15" s="27" t="n"/>
+      <c r="C15" s="21" t="inlineStr">
         <is>
           <t>09:50-11:10</t>
         </is>
       </c>
-      <c r="D15" s="1" t="inlineStr">
-        <is>
-          <t>Пусто</t>
-        </is>
-      </c>
-      <c r="E15" s="1" t="n"/>
-      <c r="F15" s="1" t="n"/>
-      <c r="G15" s="1" t="n"/>
-      <c r="H15" s="1" t="n"/>
+      <c r="D15" s="6" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
+      <c r="E15" s="22" t="n"/>
     </row>
     <row r="16">
-      <c r="B16" s="1" t="n"/>
-      <c r="C16" s="1" t="inlineStr">
+      <c r="B16" s="27" t="n"/>
+      <c r="C16" s="21" t="inlineStr">
         <is>
           <t>11:25-12:45</t>
         </is>
       </c>
-      <c r="D16" s="1" t="inlineStr">
-        <is>
-          <t>Пусто</t>
-        </is>
-      </c>
-      <c r="E16" s="1" t="n"/>
-      <c r="F16" s="1" t="n"/>
-      <c r="G16" s="1" t="n"/>
-      <c r="H16" s="1" t="n"/>
+      <c r="D16" s="6" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
+      <c r="E16" s="22" t="n"/>
     </row>
     <row r="17">
-      <c r="B17" s="1" t="n"/>
-      <c r="C17" s="1" t="inlineStr">
+      <c r="B17" s="27" t="n"/>
+      <c r="C17" s="21" t="inlineStr">
         <is>
           <t>13:15-14:35</t>
         </is>
       </c>
-      <c r="D17" s="1" t="inlineStr">
-        <is>
-          <t>Пусто</t>
-        </is>
-      </c>
-      <c r="E17" s="1" t="n"/>
-      <c r="F17" s="1" t="n"/>
-      <c r="G17" s="1" t="n"/>
-      <c r="H17" s="1" t="n"/>
+      <c r="D17" s="6" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
+      <c r="E17" s="22" t="n"/>
     </row>
     <row r="18">
-      <c r="B18" s="1" t="n"/>
-      <c r="C18" s="1" t="inlineStr">
+      <c r="B18" s="27" t="n"/>
+      <c r="C18" s="21" t="inlineStr">
         <is>
           <t>14:50-16:10</t>
         </is>
       </c>
-      <c r="D18" s="1" t="inlineStr">
-        <is>
-          <t>Пусто</t>
-        </is>
-      </c>
-      <c r="E18" s="1" t="n"/>
-      <c r="F18" s="1" t="n"/>
-      <c r="G18" s="1" t="n"/>
-      <c r="H18" s="1" t="n"/>
+      <c r="D18" s="6" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
+      <c r="E18" s="22" t="n"/>
     </row>
     <row r="19">
-      <c r="B19" s="1" t="n"/>
-      <c r="C19" s="1" t="inlineStr">
+      <c r="B19" s="27" t="n"/>
+      <c r="C19" s="21" t="inlineStr">
         <is>
           <t>16:40-18:00</t>
         </is>
       </c>
-      <c r="D19" s="1" t="inlineStr">
-        <is>
-          <t>Пусто</t>
-        </is>
-      </c>
-      <c r="E19" s="1" t="n"/>
-      <c r="F19" s="1" t="n"/>
-      <c r="G19" s="1" t="n"/>
-      <c r="H19" s="1" t="n"/>
-    </row>
-    <row r="20">
-      <c r="B20" s="1" t="n"/>
-      <c r="C20" s="1" t="inlineStr">
+      <c r="D19" s="6" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
+      <c r="E19" s="22" t="n"/>
+    </row>
+    <row r="20" ht="15.75" customHeight="1" s="1" thickBot="1">
+      <c r="B20" s="28" t="n"/>
+      <c r="C20" s="23" t="inlineStr">
         <is>
           <t>18:10-19:30</t>
         </is>
       </c>
-      <c r="D20" s="1" t="inlineStr">
-        <is>
-          <t>Пусто</t>
-        </is>
-      </c>
-      <c r="E20" s="1" t="n"/>
-      <c r="F20" s="1" t="n"/>
-      <c r="G20" s="1" t="n"/>
-      <c r="H20" s="1" t="n"/>
-    </row>
-    <row r="21">
-      <c r="B21" s="1" t="n"/>
-      <c r="C21" s="1" t="n"/>
-      <c r="D21" s="1" t="n"/>
-      <c r="E21" s="1" t="n"/>
-      <c r="F21" s="1" t="n"/>
-      <c r="G21" s="1" t="n"/>
-      <c r="H21" s="1" t="n"/>
-    </row>
+      <c r="D20" s="24" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
+      <c r="E20" s="25" t="n"/>
+    </row>
+    <row r="21" ht="3.75" customHeight="1" s="1"/>
+    <row r="22" ht="3.75" customHeight="1" s="1"/>
+    <row r="23" ht="3.75" customHeight="1" s="1" thickBot="1"/>
     <row r="24">
-      <c r="C24" t="inlineStr">
+      <c r="B24" s="26" t="inlineStr">
+        <is>
+          <t>СРЕДА</t>
+        </is>
+      </c>
+      <c r="C24" s="18" t="inlineStr">
         <is>
           <t>08:15-09:35</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>Пусто</t>
-        </is>
-      </c>
+      <c r="D24" s="19" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
+      <c r="E24" s="20" t="n"/>
     </row>
     <row r="25">
-      <c r="C25" t="inlineStr">
+      <c r="B25" s="27" t="n"/>
+      <c r="C25" s="21" t="inlineStr">
         <is>
           <t>09:50-11:10</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>Пусто</t>
-        </is>
-      </c>
+      <c r="D25" s="6" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
+      <c r="E25" s="22" t="n"/>
     </row>
     <row r="26">
-      <c r="C26" t="inlineStr">
+      <c r="B26" s="27" t="n"/>
+      <c r="C26" s="21" t="inlineStr">
         <is>
           <t>11:25-12:45</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>Пусто</t>
-        </is>
-      </c>
+      <c r="D26" s="6" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
+      <c r="E26" s="22" t="n"/>
     </row>
     <row r="27">
-      <c r="C27" t="inlineStr">
+      <c r="B27" s="27" t="n"/>
+      <c r="C27" s="21" t="inlineStr">
         <is>
           <t>13:15-14:35</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>Пусто</t>
-        </is>
-      </c>
+      <c r="D27" s="6" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
+      <c r="E27" s="22" t="n"/>
     </row>
     <row r="28">
-      <c r="C28" t="inlineStr">
+      <c r="B28" s="27" t="n"/>
+      <c r="C28" s="21" t="inlineStr">
         <is>
           <t>14:50-16:10</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>Пусто</t>
-        </is>
-      </c>
+      <c r="D28" s="6" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
+      <c r="E28" s="22" t="n"/>
     </row>
     <row r="29">
-      <c r="C29" t="inlineStr">
+      <c r="B29" s="27" t="n"/>
+      <c r="C29" s="21" t="inlineStr">
         <is>
           <t>16:40-18:00</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>Пусто</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="C30" t="inlineStr">
+      <c r="D29" s="6" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
+      <c r="E29" s="22" t="n"/>
+    </row>
+    <row r="30" ht="15.75" customHeight="1" s="1" thickBot="1">
+      <c r="B30" s="28" t="n"/>
+      <c r="C30" s="23" t="inlineStr">
         <is>
           <t>18:10-19:30</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>Пусто</t>
-        </is>
-      </c>
-    </row>
+      <c r="D30" s="24" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
+      <c r="E30" s="25" t="n"/>
+    </row>
+    <row r="31" ht="3" customHeight="1" s="1"/>
+    <row r="32" ht="3" customHeight="1" s="1"/>
+    <row r="33" ht="4.5" customHeight="1" s="1" thickBot="1"/>
     <row r="34">
-      <c r="C34" t="inlineStr">
+      <c r="B34" s="26" t="inlineStr">
+        <is>
+          <t>ЧЕТВЕРГ</t>
+        </is>
+      </c>
+      <c r="C34" s="18" t="inlineStr">
         <is>
           <t>08:15-09:35</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>Пусто</t>
-        </is>
-      </c>
+      <c r="D34" s="19" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
+      <c r="E34" s="20" t="n"/>
     </row>
     <row r="35">
-      <c r="C35" t="inlineStr">
+      <c r="B35" s="27" t="n"/>
+      <c r="C35" s="21" t="inlineStr">
         <is>
           <t>09:50-11:10</t>
         </is>
       </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>Пусто</t>
-        </is>
-      </c>
+      <c r="D35" s="6" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
+      <c r="E35" s="22" t="n"/>
     </row>
     <row r="36">
-      <c r="C36" t="inlineStr">
+      <c r="B36" s="27" t="n"/>
+      <c r="C36" s="21" t="inlineStr">
         <is>
           <t>11:25-12:45</t>
         </is>
       </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>Пусто</t>
-        </is>
-      </c>
+      <c r="D36" s="6" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
+      <c r="E36" s="22" t="n"/>
     </row>
     <row r="37">
-      <c r="C37" t="inlineStr">
+      <c r="B37" s="27" t="n"/>
+      <c r="C37" s="21" t="inlineStr">
         <is>
           <t>13:15-14:35</t>
         </is>
       </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>Пусто</t>
-        </is>
-      </c>
+      <c r="D37" s="6" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
+      <c r="E37" s="22" t="n"/>
     </row>
     <row r="38">
-      <c r="C38" t="inlineStr">
+      <c r="B38" s="27" t="n"/>
+      <c r="C38" s="21" t="inlineStr">
         <is>
           <t>14:50-16:10</t>
         </is>
       </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>Пусто</t>
-        </is>
-      </c>
+      <c r="D38" s="6" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
+      <c r="E38" s="22" t="n"/>
     </row>
     <row r="39">
-      <c r="C39" t="inlineStr">
+      <c r="B39" s="27" t="n"/>
+      <c r="C39" s="21" t="inlineStr">
         <is>
           <t>16:40-18:00</t>
         </is>
       </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>Пусто</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="C40" t="inlineStr">
+      <c r="D39" s="6" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
+      <c r="E39" s="22" t="n"/>
+    </row>
+    <row r="40" ht="15.75" customHeight="1" s="1" thickBot="1">
+      <c r="B40" s="28" t="n"/>
+      <c r="C40" s="23" t="inlineStr">
         <is>
           <t>18:10-19:30</t>
         </is>
       </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>Пусто</t>
-        </is>
-      </c>
-    </row>
+      <c r="D40" s="24" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
+      <c r="E40" s="25" t="n"/>
+    </row>
+    <row r="41" ht="3.75" customHeight="1" s="1"/>
+    <row r="42" ht="3.75" customHeight="1" s="1"/>
+    <row r="43" ht="3" customHeight="1" s="1" thickBot="1"/>
     <row r="44">
-      <c r="C44" t="inlineStr">
+      <c r="B44" s="26" t="inlineStr">
+        <is>
+          <t>ПЯТНИЦА</t>
+        </is>
+      </c>
+      <c r="C44" s="18" t="inlineStr">
         <is>
           <t>08:15-09:35</t>
         </is>
       </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>Пусто</t>
-        </is>
-      </c>
+      <c r="D44" s="19" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
+      <c r="E44" s="20" t="n"/>
     </row>
     <row r="45">
-      <c r="C45" t="inlineStr">
+      <c r="B45" s="27" t="n"/>
+      <c r="C45" s="21" t="inlineStr">
         <is>
           <t>09:50-11:10</t>
         </is>
       </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>Пусто</t>
-        </is>
-      </c>
+      <c r="D45" s="6" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
+      <c r="E45" s="22" t="n"/>
     </row>
     <row r="46">
-      <c r="C46" t="inlineStr">
+      <c r="B46" s="27" t="n"/>
+      <c r="C46" s="21" t="inlineStr">
         <is>
           <t>11:25-12:45</t>
         </is>
       </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>Пусто</t>
-        </is>
-      </c>
+      <c r="D46" s="6" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
+      <c r="E46" s="22" t="n"/>
     </row>
     <row r="47">
-      <c r="C47" t="inlineStr">
+      <c r="B47" s="27" t="n"/>
+      <c r="C47" s="21" t="inlineStr">
         <is>
           <t>13:15-14:35</t>
         </is>
       </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>Пусто</t>
-        </is>
-      </c>
+      <c r="D47" s="6" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
+      <c r="E47" s="22" t="n"/>
     </row>
     <row r="48">
-      <c r="C48" t="inlineStr">
+      <c r="B48" s="27" t="n"/>
+      <c r="C48" s="21" t="inlineStr">
         <is>
           <t>14:50-16:10</t>
         </is>
       </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>Пусто</t>
-        </is>
-      </c>
+      <c r="D48" s="6" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
+      <c r="E48" s="22" t="n"/>
     </row>
     <row r="49">
-      <c r="C49" t="inlineStr">
+      <c r="B49" s="27" t="n"/>
+      <c r="C49" s="21" t="inlineStr">
         <is>
           <t>16:40-18:00</t>
         </is>
       </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>Пусто</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="C50" t="inlineStr">
+      <c r="D49" s="6" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
+      <c r="E49" s="22" t="n"/>
+    </row>
+    <row r="50" ht="15.75" customHeight="1" s="1" thickBot="1">
+      <c r="B50" s="28" t="n"/>
+      <c r="C50" s="23" t="inlineStr">
         <is>
           <t>18:10-19:30</t>
         </is>
       </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>Пусто</t>
-        </is>
-      </c>
-    </row>
+      <c r="D50" s="24" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
+      <c r="E50" s="25" t="n"/>
+    </row>
+    <row r="51" ht="3" customHeight="1" s="1"/>
+    <row r="52" ht="3.75" customHeight="1" s="1"/>
+    <row r="53" ht="4.5" customHeight="1" s="1" thickBot="1"/>
     <row r="54">
-      <c r="C54" t="inlineStr">
+      <c r="B54" s="26" t="inlineStr">
+        <is>
+          <t>СУББОТА</t>
+        </is>
+      </c>
+      <c r="C54" s="18" t="inlineStr">
         <is>
           <t>08:15-09:35</t>
         </is>
       </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>Пусто</t>
-        </is>
-      </c>
+      <c r="D54" s="19" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
+      <c r="E54" s="20" t="n"/>
     </row>
     <row r="55">
-      <c r="C55" t="inlineStr">
+      <c r="B55" s="27" t="n"/>
+      <c r="C55" s="21" t="inlineStr">
         <is>
           <t>09:50-11:10</t>
         </is>
       </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>Пусто</t>
-        </is>
-      </c>
+      <c r="D55" s="6" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
+      <c r="E55" s="22" t="n"/>
     </row>
     <row r="56">
-      <c r="C56" t="inlineStr">
+      <c r="B56" s="27" t="n"/>
+      <c r="C56" s="21" t="inlineStr">
         <is>
           <t>11:25-12:45</t>
         </is>
       </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>Пусто</t>
-        </is>
-      </c>
+      <c r="D56" s="6" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
+      <c r="E56" s="22" t="n"/>
     </row>
     <row r="57">
-      <c r="C57" t="inlineStr">
+      <c r="B57" s="27" t="n"/>
+      <c r="C57" s="21" t="inlineStr">
         <is>
           <t>13:15-14:35</t>
         </is>
       </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>Пусто</t>
-        </is>
-      </c>
+      <c r="D57" s="6" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
+      <c r="E57" s="22" t="n"/>
     </row>
     <row r="58">
-      <c r="C58" t="inlineStr">
+      <c r="B58" s="27" t="n"/>
+      <c r="C58" s="21" t="inlineStr">
         <is>
           <t>14:50-16:10</t>
         </is>
       </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>Пусто</t>
-        </is>
-      </c>
+      <c r="D58" s="6" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
+      <c r="E58" s="22" t="n"/>
     </row>
     <row r="59">
-      <c r="C59" t="inlineStr">
+      <c r="B59" s="27" t="n"/>
+      <c r="C59" s="21" t="inlineStr">
         <is>
           <t>16:40-18:00</t>
         </is>
       </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>Пусто</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="C60" t="inlineStr">
+      <c r="D59" s="6" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
+      <c r="E59" s="22" t="n"/>
+    </row>
+    <row r="60" ht="15.75" customHeight="1" s="1" thickBot="1">
+      <c r="B60" s="28" t="n"/>
+      <c r="C60" s="23" t="inlineStr">
         <is>
           <t>18:10-19:30</t>
         </is>
       </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>Пусто</t>
-        </is>
-      </c>
+      <c r="D60" s="24" t="inlineStr">
+        <is>
+          <t>Пусто</t>
+        </is>
+      </c>
+      <c r="E60" s="25" t="n"/>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B44:B50"/>
+    <mergeCell ref="B24:B30"/>
+    <mergeCell ref="B4:B10"/>
+    <mergeCell ref="B34:B40"/>
+    <mergeCell ref="B54:B60"/>
+    <mergeCell ref="B14:B20"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
AUTO FROM work 13.06.2024 14:24:36,61
</commit_message>
<xml_diff>
--- a/media/1.xlsx
+++ b/media/1.xlsx
@@ -661,16 +661,8 @@
           <t>08:15-09:35</t>
         </is>
       </c>
-      <c r="D4" s="19" t="inlineStr">
-        <is>
-          <t>Разр. ПО для моб. Платформ ФМЕ ПОИТ3 ЗФПО</t>
-        </is>
-      </c>
-      <c r="E4" s="20" t="inlineStr">
-        <is>
-          <t>210</t>
-        </is>
-      </c>
+      <c r="D4" s="19" t="inlineStr"/>
+      <c r="E4" s="20" t="n"/>
     </row>
     <row r="5">
       <c r="B5" s="27" t="n"/>
@@ -681,10 +673,14 @@
       </c>
       <c r="D5" s="6" t="inlineStr">
         <is>
-          <t>Резерв</t>
-        </is>
-      </c>
-      <c r="E5" s="22" t="n"/>
+          <t>СПП (ЗО) 2 курс ФМЕ ПОИТ3 ЗФПО</t>
+        </is>
+      </c>
+      <c r="E5" s="22" t="inlineStr">
+        <is>
+          <t>364</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="B6" s="27" t="n"/>
@@ -695,12 +691,12 @@
       </c>
       <c r="D6" s="6" t="inlineStr">
         <is>
-          <t>СПП (ЗО) 2 курс колония</t>
+          <t>СПП (ЗО) 2 курс ФМЕ ПОИТ3 ЗФПО</t>
         </is>
       </c>
       <c r="E6" s="22" t="inlineStr">
         <is>
-          <t>115</t>
+          <t>364</t>
         </is>
       </c>
     </row>
@@ -758,8 +754,16 @@
           <t>08:15-09:35</t>
         </is>
       </c>
-      <c r="D14" s="19" t="inlineStr"/>
-      <c r="E14" s="20" t="n"/>
+      <c r="D14" s="19" t="inlineStr">
+        <is>
+          <t>СПП (ЗО) 2 курс ФМЕ ПОИТ3 ЗФПО</t>
+        </is>
+      </c>
+      <c r="E14" s="20" t="inlineStr">
+        <is>
+          <t>364</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="B15" s="27" t="n"/>
@@ -768,8 +772,16 @@
           <t>09:50-11:10</t>
         </is>
       </c>
-      <c r="D15" s="6" t="inlineStr"/>
-      <c r="E15" s="22" t="n"/>
+      <c r="D15" s="6" t="inlineStr">
+        <is>
+          <t>СПП (ЗО) 2 курс ФМЕ ПОИТ3 ЗФПО</t>
+        </is>
+      </c>
+      <c r="E15" s="22" t="inlineStr">
+        <is>
+          <t>364</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="B16" s="27" t="n"/>
@@ -778,8 +790,16 @@
           <t>11:25-12:45</t>
         </is>
       </c>
-      <c r="D16" s="6" t="inlineStr"/>
-      <c r="E16" s="22" t="n"/>
+      <c r="D16" s="6" t="inlineStr">
+        <is>
+          <t>Разр. ПО для моб. Платформ ФМЕ ПОИТ3 ЗФПО</t>
+        </is>
+      </c>
+      <c r="E16" s="22" t="inlineStr">
+        <is>
+          <t>364</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="B17" s="27" t="n"/>
@@ -835,8 +855,16 @@
           <t>08:15-09:35</t>
         </is>
       </c>
-      <c r="D24" s="19" t="inlineStr"/>
-      <c r="E24" s="20" t="n"/>
+      <c r="D24" s="19" t="inlineStr">
+        <is>
+          <t>Разр. ПО для моб. Платформ ФМЕ ПОИТ3 ЗФПО</t>
+        </is>
+      </c>
+      <c r="E24" s="20" t="inlineStr">
+        <is>
+          <t>364</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="B25" s="27" t="n"/>
@@ -912,8 +940,16 @@
           <t>08:15-09:35</t>
         </is>
       </c>
-      <c r="D34" s="19" t="inlineStr"/>
-      <c r="E34" s="20" t="n"/>
+      <c r="D34" s="19" t="inlineStr">
+        <is>
+          <t>СПП (ЗО) 2 курс ФМЕ ПОИТ3 ЗФПО</t>
+        </is>
+      </c>
+      <c r="E34" s="20" t="inlineStr">
+        <is>
+          <t>364</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="B35" s="27" t="n"/>
@@ -922,8 +958,16 @@
           <t>09:50-11:10</t>
         </is>
       </c>
-      <c r="D35" s="6" t="inlineStr"/>
-      <c r="E35" s="22" t="n"/>
+      <c r="D35" s="6" t="inlineStr">
+        <is>
+          <t>СПП (ЗО) 2 курс ФМЕ ПОИТ3 ЗФПО</t>
+        </is>
+      </c>
+      <c r="E35" s="22" t="inlineStr">
+        <is>
+          <t>364</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="B36" s="27" t="n"/>
@@ -932,8 +976,16 @@
           <t>11:25-12:45</t>
         </is>
       </c>
-      <c r="D36" s="6" t="inlineStr"/>
-      <c r="E36" s="22" t="n"/>
+      <c r="D36" s="6" t="inlineStr">
+        <is>
+          <t>СПП (ЗО) 2 курс ФМЕ ПОИТ3 ЗФПО</t>
+        </is>
+      </c>
+      <c r="E36" s="22" t="inlineStr">
+        <is>
+          <t>364</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="B37" s="27" t="n"/>
@@ -1009,8 +1061,16 @@
           <t>11:25-12:45</t>
         </is>
       </c>
-      <c r="D46" s="6" t="inlineStr"/>
-      <c r="E46" s="22" t="n"/>
+      <c r="D46" s="6" t="inlineStr">
+        <is>
+          <t>СПП (ЗО) 2 курс ФМЕ ПОИТ3 ЗФПО</t>
+        </is>
+      </c>
+      <c r="E46" s="22" t="inlineStr">
+        <is>
+          <t>364</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="B47" s="27" t="n"/>
@@ -1019,8 +1079,16 @@
           <t>13:15-14:35</t>
         </is>
       </c>
-      <c r="D47" s="6" t="inlineStr"/>
-      <c r="E47" s="22" t="n"/>
+      <c r="D47" s="6" t="inlineStr">
+        <is>
+          <t>СПП (ЗО) 2 курс ФМЕ ПОИТ3 ЗФПО</t>
+        </is>
+      </c>
+      <c r="E47" s="22" t="inlineStr">
+        <is>
+          <t>364</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="B48" s="27" t="n"/>
@@ -1029,8 +1097,16 @@
           <t>14:50-16:10</t>
         </is>
       </c>
-      <c r="D48" s="6" t="inlineStr"/>
-      <c r="E48" s="22" t="n"/>
+      <c r="D48" s="6" t="inlineStr">
+        <is>
+          <t>СПП (ЗО) 2 курс ФМЕ ПОИТ3 ЗФПО</t>
+        </is>
+      </c>
+      <c r="E48" s="22" t="inlineStr">
+        <is>
+          <t>364</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="B49" s="27" t="n"/>

</xml_diff>